<commit_message>
Aanpassingen aan test beschrijving aanpassing aan testbestanden oude bestanden verwijderd nieuwe toegevoegd
</commit_message>
<xml_diff>
--- a/catalogusdata/Logische testen Catalogus Wessel.xlsx
+++ b/catalogusdata/Logische testen Catalogus Wessel.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$D$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>US</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Testbestand wordt geupload</t>
   </si>
   <si>
-    <t>Bij start test is er geen data aanwezig</t>
-  </si>
-  <si>
     <t>Ingelogde gebruiker</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t>Testbestand is geupload</t>
   </si>
   <si>
-    <t>Testbestand wordt nogmaals geupload</t>
-  </si>
-  <si>
     <t>GCO-540</t>
   </si>
   <si>
@@ -73,43 +67,69 @@
     <t xml:space="preserve">Testbestand wordt geupload </t>
   </si>
   <si>
-    <t xml:space="preserve"> Via menu navigeren naar Over en vervolgens in de dropdown Catalogus selecteren. Catalogus informatie wordt zichtbaar</t>
-  </si>
-  <si>
-    <t>http://data.test.pdok.nl/catalogus/dso/doc/catalogus/DigitaalStelselOmgevingswet geeft data terug.</t>
-  </si>
-  <si>
-    <t>Laatste activiteit is bijgewerkt</t>
-  </si>
-  <si>
     <t>GCO-526</t>
   </si>
   <si>
-    <t>http://data.test.pdok.nl/catalogus/dso/query/overzichtdatasets toont in het overzicht de dataset van de OmgevingsWet</t>
-  </si>
-  <si>
-    <t>Dataset OW T.ttl</t>
-  </si>
-  <si>
-    <t>Test bestand wordt aangepast rdfs:label veranderd van "omgevingswet" naar "dataset omgevingswet"</t>
-  </si>
-  <si>
-    <t>Dataset BAL T.ttl</t>
-  </si>
-  <si>
-    <t>Testresultaten van stap 4 en 5 zijn nog aanweizg</t>
-  </si>
-  <si>
-    <t>/overzichtdatasets toont in het overzicht de dataset van de omgevingswet maar nu met het label "dataset omgevingswet"</t>
-  </si>
-  <si>
-    <t>/overzichtdatasets toont in het overzicht naast de dataset van de Omgevingswet nu ook de toegevoegde dataset van het BAL</t>
-  </si>
-  <si>
-    <t>wacht 5 minuten</t>
-  </si>
-  <si>
-    <t>/overzcihtdatasets toont nog steeds twee datasets. Selecteer de BAL dataset en merk op dat de laatste activiteit niet is bijgewerkt aangezien er geen wijzigingen aan het bestand zijn aangebracht</t>
+    <t>Onderwerp</t>
+  </si>
+  <si>
+    <t>Testnaam</t>
+  </si>
+  <si>
+    <t>Catalogus put ttl</t>
+  </si>
+  <si>
+    <t>Upload controle</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Container geeft als resultaat "Upload succesvol"</t>
+  </si>
+  <si>
+    <t>Datacontrole attributen</t>
+  </si>
+  <si>
+    <t>Pagina /catalogus/dso/doc/catalogus/Test wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave met als header 'Test Catalogus'
+In de tabel staan o.a. de volgende rijen (header | waarde):
+- Titel | Test Catalogus
+- Beschrijving | Een Catalogus voor Testdoeleinden</t>
+  </si>
+  <si>
+    <t>Dataset T.ttl</t>
+  </si>
+  <si>
+    <t>Pagina /catalogus/dso/query/overzichtdatasets wordt bekeken</t>
+  </si>
+  <si>
+    <t>Op de pagina is o.a. het volgende te zien:
+- Tabelweergave
+In de tabel staat o.a. de volgende rij (header | waarde):
+- dataset | Testdataset
+- uitleg | Een Dataset voor Testdoeleinden</t>
+  </si>
+  <si>
+    <t>Pagina /catalogus/dso/doc/Testdataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Op de pagina is o.a. het volgende te zien: Tabelweergave met als titel "Testdataset"; Daarnaast is er een Titel | Testdataset zichtbaar, een Beschrijving | Dataset voor testdoeleinde zichtbaar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synchronisatie Controle </t>
+  </si>
+  <si>
+    <t>TestConcepten.ttl</t>
+  </si>
+  <si>
+    <t>Pagina /catalogus/dso/update/syncttlupload</t>
+  </si>
+  <si>
+    <t>Op de pagina is een upload container zichtbaar waar uit een selectie form de Testdataset geselecteerd kan worden</t>
   </si>
 </sst>
 </file>
@@ -279,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -327,6 +347,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -634,274 +660,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H405"/>
+  <dimension ref="A1:J405"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="15"/>
-    <col min="2" max="2" width="15.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" style="12" customWidth="1"/>
-    <col min="4" max="5" width="35.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="14" customWidth="1"/>
-    <col min="7" max="8" width="35.7109375" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="2" max="2" width="35.85546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="12" customWidth="1"/>
+    <col min="6" max="7" width="35.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" style="14" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="35.7109375" style="15" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="10" t="s">
+      <c r="G2" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+    </row>
+    <row r="3" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="G3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="J3" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="13" t="s">
+      <c r="G4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="F5" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="D6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="I7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="C8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="I8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>14</v>
       </c>
@@ -2852,12 +2913,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H2"/>
+  <autoFilter ref="D2:J2"/>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1"/>
-    <hyperlink ref="H6" r:id="rId2"/>
+    <hyperlink ref="J6" r:id="rId1" display="http://data.test.pdok.nl/catalogus/dso/query/overzichtdatasets toont in het overzicht de dataset van de OmgevingsWet"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>